<commit_message>
Format angepasst, Report gekürzt
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\50_Informatik\100_R\001_Kunden\TaB\Abrechnungen\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kinoclub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36E5CC3-7FEE-42B7-AD95-50F643C4443F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CB483A-9DE3-4CE0-B7B9-2A528DA78A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6552" yWindow="6552" windowWidth="15684" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -359,17 +359,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -380,7 +380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45242</v>
       </c>
@@ -388,10 +388,10 @@
         <v>1018.405</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45262</v>
       </c>
@@ -402,7 +402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45256</v>
       </c>

</xml_diff>

<commit_message>
Error handling: Verleiherabgabe nicht vorhanden
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kinoclub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoclub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CB483A-9DE3-4CE0-B7B9-2A528DA78A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9A073A-E37A-4D08-BF3F-9393A1FE7D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6552" yWindow="6552" windowWidth="15684" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -356,20 +356,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -380,7 +380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45242</v>
       </c>
@@ -391,7 +391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45262</v>
       </c>
@@ -402,7 +402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45256</v>
       </c>
@@ -410,6 +410,17 @@
         <v>1016.751</v>
       </c>
       <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45267</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1016.751</v>
+      </c>
+      <c r="C5">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Verleiherabgaben mit Fixbetrag und Kinoförderer gratis
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E47A285-BA39-44B1-85B4-0105AB250AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C5B33-DAFF-4E90-B73A-6B07ABC4C479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>Suisa</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>Kein Verleiher mehr</t>
-  </si>
-  <si>
-    <t>nicht gefunden</t>
   </si>
   <si>
     <t>Kinoförderer gratis?</t>
@@ -397,10 +394,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:B26" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:B26" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A26">
-    <sortCondition ref="A1:A58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:B25" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:B25" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A23">
+    <sortCondition ref="A1:A55"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="1"/>
@@ -686,7 +683,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,15 +1096,27 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BAA3C643-507F-407E-BA6D-AF31EB48F8B1}">
+          <x14:formula1>
+            <xm:f>'Kinoförderer gratis'!$A$2:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F25</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2012A76-D168-4BE0-9450-2E40BA8CE7CD}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,12 +1130,12 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -1134,7 +1143,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>25</v>
@@ -1221,8 +1230,8 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>60</v>
+      <c r="A14" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>25</v>
@@ -1230,7 +1239,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>25</v>
@@ -1238,39 +1247,39 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>53</v>
+      <c r="A17" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>51</v>
+      <c r="A18" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>46</v>
+      <c r="A19" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>49</v>
+      <c r="A20" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>25</v>
@@ -1278,43 +1287,35 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>42</v>
+      <c r="A22" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>41</v>
+      <c r="A23" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1328,7 +1329,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B26</xm:sqref>
+          <xm:sqref>B2:B25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1351,7 +1352,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Neue Vorstellung 22.2.24 Bergfahrt
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD6E7F0-74BA-4361-96BB-57B18B4D4748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7964EE-1BB2-4811-9749-6F82EBC2ABC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
   <si>
     <t>Suisa</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Filmcoopi Zürich AG</t>
-  </si>
-  <si>
-    <t>cineworx gmbh</t>
   </si>
   <si>
     <t>Xenix Filmdistribution GmbH</t>
@@ -898,7 +895,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -993,7 +990,7 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1090,7 +1087,7 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1110,7 +1107,7 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1243,7 +1240,7 @@
         <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1257,7 +1254,7 @@
         <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1271,7 +1268,7 @@
         <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1287,7 +1284,7 @@
         <v>32</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1315,7 +1312,7 @@
         <v>34</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1329,7 +1326,7 @@
         <v>35</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1378,7 +1375,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,84 +1392,84 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1483,13 +1480,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1500,13 +1497,13 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="9">
         <v>8057</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1517,13 +1514,13 @@
         <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1534,149 +1531,149 @@
         <v>25</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>99</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>103</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1687,47 +1684,47 @@
         <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="E18" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1773,7 +1770,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ella und der schwarze Jaguar 10.04.2024
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9566E5C-A244-45E8-946C-F5F3472D363A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076B31AD-BF5D-4D0E-B09A-AD06CE513500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>45393</v>
+        <v>45392</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>110</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>45400</v>
+        <v>45392</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>112</v>
@@ -1484,7 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2012A76-D168-4BE0-9450-2E40BA8CE7CD}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+    <sheetView zoomScale="129" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mindest Garantie für Röbi geht korrigiert
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381CB01C-606D-45F2-A294-A7FDA2BF9BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F6874A-E842-4737-91BA-D01E0A8B2CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -937,7 +937,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1324,7 @@
         <v>150</v>
       </c>
       <c r="D19" s="8">
-        <v>30</v>
+        <v>29.222840000000001</v>
       </c>
       <c r="F19" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Verleiherabgaben La Chimera weniger als 150.00 CHF MG
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB616554-DB60-4292-A363-719EE0FB234F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861865EE-6A48-4F24-8DCE-66CDB5C2477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -946,7 +946,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1370,7 @@
         <v>116</v>
       </c>
       <c r="C21" s="6">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D21" s="8">
         <v>30</v>

</xml_diff>

<commit_message>
neue Kinovorstellungen zweite Saison 2024
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861865EE-6A48-4F24-8DCE-66CDB5C2477E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4CFFA1-5705-48B9-ADB6-E6D70410D561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15288" yWindow="0" windowWidth="15528" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="164">
   <si>
     <t>Suisa</t>
   </si>
@@ -407,6 +407,129 @@
   </si>
   <si>
     <t>9999.094</t>
+  </si>
+  <si>
+    <t>1017.788</t>
+  </si>
+  <si>
+    <t>Wow! Nachricht aus dem All</t>
+  </si>
+  <si>
+    <t>1020.078</t>
+  </si>
+  <si>
+    <t>Zwei zu Eins</t>
+  </si>
+  <si>
+    <t>1019.700</t>
+  </si>
+  <si>
+    <t>Die Herrlichkeit des Lebens</t>
+  </si>
+  <si>
+    <t>1020.051</t>
+  </si>
+  <si>
+    <t>MUSIK: Resilient Man</t>
+  </si>
+  <si>
+    <t>1017.067</t>
+  </si>
+  <si>
+    <t>La Passion de Dodin Bouffant</t>
+  </si>
+  <si>
+    <t>1020.576</t>
+  </si>
+  <si>
+    <t>Tschugger - De Lätscht Fall</t>
+  </si>
+  <si>
+    <t>1019.820</t>
+  </si>
+  <si>
+    <t>FAMILIE: Die Schule der Magischen Tieren 3</t>
+  </si>
+  <si>
+    <t>1019.485</t>
+  </si>
+  <si>
+    <t>The Monk and the Gun</t>
+  </si>
+  <si>
+    <t>1019.043</t>
+  </si>
+  <si>
+    <t>MUSIK: Margini</t>
+  </si>
+  <si>
+    <t>1016.779</t>
+  </si>
+  <si>
+    <t>FAMILIE: Harold und die Zauberkreide</t>
+  </si>
+  <si>
+    <t>1019.776</t>
+  </si>
+  <si>
+    <t>MUSIK: Bolero</t>
+  </si>
+  <si>
+    <t>1014.761</t>
+  </si>
+  <si>
+    <t>Denkanstoss: Scent of Fear</t>
+  </si>
+  <si>
+    <t>1020.552</t>
+  </si>
+  <si>
+    <t>Kalbermatten</t>
+  </si>
+  <si>
+    <t>1005.027</t>
+  </si>
+  <si>
+    <t>TANGONACHT</t>
+  </si>
+  <si>
+    <t>1020.295</t>
+  </si>
+  <si>
+    <t>Die Tabubrecherin</t>
+  </si>
+  <si>
+    <t>1019.044</t>
+  </si>
+  <si>
+    <t>MUSIK: Joan Baez</t>
+  </si>
+  <si>
+    <t>FAMILIE: Weihnachtsfilm</t>
+  </si>
+  <si>
+    <t>1020.399</t>
+  </si>
+  <si>
+    <t>Der Buchspazierer</t>
+  </si>
+  <si>
+    <t>Garfield De Film</t>
+  </si>
+  <si>
+    <t>Sony Pictures Releasing Switzerland GmbH</t>
+  </si>
+  <si>
+    <t>Frenetic Films AG</t>
+  </si>
+  <si>
+    <t>Ascot Elite</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>Langjahr Film GmbH</t>
   </si>
 </sst>
 </file>
@@ -416,7 +539,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +573,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -459,7 +589,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -467,11 +597,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -488,11 +631,25 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -612,18 +769,6 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -638,33 +783,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:G25" totalsRowShown="0">
-  <autoFilter ref="A1:G25" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:G45" totalsRowShown="0">
+  <autoFilter ref="A1:G45" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{056159D4-E39B-4BCA-A63C-616B27132666}" name="Abzug [%]"/>
     <tableColumn id="4" xr3:uid="{3889FFD6-1D01-42CF-9D0C-73A343093947}" name="Abzug fix [CHF]"/>
     <tableColumn id="6" xr3:uid="{7EA53B63-9001-4ABE-801A-79A1AD834F4D}" name="Titel"/>
-    <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:E21" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A19">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{C3C9F269-200E-44AA-A999-C80DE0337772}" name="Kinoförderer gratis?" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A3438286-188F-4B22-96EA-9046C8BD8738}" name="Adresse" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{4E36D4B9-CEC6-4204-8ACA-9F0B34AACC27}" name="PLZ" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{9871F211-6A68-4A87-B2B5-D2BD49D8C28F}" name="Ort" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C3C9F269-200E-44AA-A999-C80DE0337772}" name="Kinoförderer gratis?" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{A3438286-188F-4B22-96EA-9046C8BD8738}" name="Adresse" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4E36D4B9-CEC6-4204-8ACA-9F0B34AACC27}" name="PLZ" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9871F211-6A68-4A87-B2B5-D2BD49D8C28F}" name="Ort" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -943,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,6 +1604,380 @@
       </c>
       <c r="G25" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45512</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="F26" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45543</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1017.341</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>158</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45555</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="6">
+        <v>150</v>
+      </c>
+      <c r="D28" s="8">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45557</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="6">
+        <v>150</v>
+      </c>
+      <c r="D29" s="8">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45562</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="6">
+        <v>150</v>
+      </c>
+      <c r="D30" s="8">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45571</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="6">
+        <v>150</v>
+      </c>
+      <c r="D31" s="8">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45576</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="6">
+        <v>150</v>
+      </c>
+      <c r="D32" s="8">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45577</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="6">
+        <v>150</v>
+      </c>
+      <c r="D33" s="8">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45578</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="6">
+        <v>150</v>
+      </c>
+      <c r="D34" s="8">
+        <v>50</v>
+      </c>
+      <c r="F34" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>45583</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="6">
+        <v>150</v>
+      </c>
+      <c r="D35" s="8">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>45590</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="6">
+        <v>200</v>
+      </c>
+      <c r="D36" s="8">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45599</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="6">
+        <v>150</v>
+      </c>
+      <c r="D37" s="8">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
+        <v>142</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>45604</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="6">
+        <v>150</v>
+      </c>
+      <c r="D38" s="8">
+        <v>30</v>
+      </c>
+      <c r="F38" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>45606</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="6">
+        <v>150</v>
+      </c>
+      <c r="D39" s="8">
+        <v>30</v>
+      </c>
+      <c r="F39" t="s">
+        <v>146</v>
+      </c>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>45625</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="F40" t="s">
+        <v>148</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>45634</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="6">
+        <v>150</v>
+      </c>
+      <c r="D42" s="8">
+        <v>30</v>
+      </c>
+      <c r="F42" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>45633</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="6">
+        <v>150</v>
+      </c>
+      <c r="D43" s="8">
+        <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>154</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>45641</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="F44" t="s">
+        <v>155</v>
+      </c>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>45646</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="6">
+        <v>150</v>
+      </c>
+      <c r="D45" s="8">
+        <v>30</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45" t="s">
+        <v>157</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filmabrechnung Die Herrlichkeit des Lebens
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4CFFA1-5705-48B9-ADB6-E6D70410D561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362E1C93-1E22-4455-9F3F-A0274B4B2AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15288" yWindow="0" windowWidth="15528" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -632,24 +632,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -769,6 +756,18 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -786,30 +785,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:G45" totalsRowShown="0">
   <autoFilter ref="A1:G45" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{056159D4-E39B-4BCA-A63C-616B27132666}" name="Abzug [%]"/>
     <tableColumn id="4" xr3:uid="{3889FFD6-1D01-42CF-9D0C-73A343093947}" name="Abzug fix [CHF]"/>
     <tableColumn id="6" xr3:uid="{7EA53B63-9001-4ABE-801A-79A1AD834F4D}" name="Titel"/>
-    <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E21" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A19">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C3C9F269-200E-44AA-A999-C80DE0337772}" name="Kinoförderer gratis?" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{A3438286-188F-4B22-96EA-9046C8BD8738}" name="Adresse" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4E36D4B9-CEC6-4204-8ACA-9F0B34AACC27}" name="PLZ" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{9871F211-6A68-4A87-B2B5-D2BD49D8C28F}" name="Ort" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{C3C9F269-200E-44AA-A999-C80DE0337772}" name="Kinoförderer gratis?" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A3438286-188F-4B22-96EA-9046C8BD8738}" name="Adresse" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4E36D4B9-CEC6-4204-8ACA-9F0B34AACC27}" name="PLZ" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{9871F211-6A68-4A87-B2B5-D2BD49D8C28F}" name="Ort" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1091,7 +1090,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1616,7 @@
       <c r="F26" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1637,7 +1636,7 @@
       <c r="F27" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1657,7 +1656,7 @@
       <c r="F28" t="s">
         <v>126</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1677,7 +1676,7 @@
       <c r="F29" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1697,7 +1696,7 @@
       <c r="F30" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1717,7 +1716,7 @@
       <c r="F31" t="s">
         <v>132</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1737,7 +1736,7 @@
       <c r="F32" t="s">
         <v>134</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1757,7 +1756,7 @@
       <c r="F33" t="s">
         <v>134</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1777,7 +1776,7 @@
       <c r="F34" t="s">
         <v>136</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1797,7 +1796,7 @@
       <c r="F35" t="s">
         <v>138</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1817,7 +1816,7 @@
       <c r="F36" t="s">
         <v>140</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1837,7 +1836,7 @@
       <c r="F37" t="s">
         <v>142</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1857,7 +1856,7 @@
       <c r="F38" t="s">
         <v>144</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1877,7 +1876,6 @@
       <c r="F39" t="s">
         <v>146</v>
       </c>
-      <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
@@ -1890,7 +1888,7 @@
       <c r="F40" t="s">
         <v>148</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G40" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1905,7 +1903,7 @@
       <c r="F41" t="s">
         <v>150</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1925,7 +1923,7 @@
       <c r="F42" t="s">
         <v>152</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1945,7 +1943,7 @@
       <c r="F43" t="s">
         <v>154</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G43" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1957,7 +1955,6 @@
       <c r="F44" t="s">
         <v>155</v>
       </c>
-      <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -1976,7 +1973,7 @@
       <c r="F45" t="s">
         <v>157</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G45" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New column for distribution of costs
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5AA47F-1092-46F3-84E1-B01B047F58D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70171F1A-6E65-453B-9435-70DB056B3591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="167">
   <si>
     <t>Suisa</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>Root</t>
+  </si>
+  <si>
+    <t>Link Datum</t>
   </si>
 </sst>
 </file>
@@ -637,13 +640,13 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <b val="0"/>
@@ -775,6 +778,9 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -789,13 +795,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:G45" totalsRowShown="0">
-  <autoFilter ref="A1:G45" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:H45" totalsRowShown="0">
+  <autoFilter ref="A1:H45" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H45">
     <sortCondition ref="A1:A45"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="9"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{24D1648B-5A84-48EC-B2C9-2CE415C3BDE9}" name="Link Datum" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{056159D4-E39B-4BCA-A63C-616B27132666}" name="Abzug [%]"/>
@@ -1097,902 +1104,964 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
-    <col min="6" max="6" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45311</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6">
-        <v>150</v>
-      </c>
-      <c r="D2" s="8">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="6">
+        <v>150</v>
+      </c>
+      <c r="E2" s="8">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45312</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6">
-        <v>150</v>
-      </c>
-      <c r="D3" s="8">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" s="6">
+        <v>150</v>
+      </c>
+      <c r="E3" s="8">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45316</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6">
-        <v>150</v>
-      </c>
-      <c r="D4" s="8">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="6">
+        <v>150</v>
+      </c>
+      <c r="E4" s="8">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45319</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6">
-        <v>150</v>
-      </c>
-      <c r="D5" s="8">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="6">
+        <v>150</v>
+      </c>
+      <c r="E5" s="8">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45332</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
-        <v>150</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
+        <v>150</v>
+      </c>
+      <c r="E6" s="8">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45333</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6">
-        <v>150</v>
-      </c>
-      <c r="D7" s="8">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D7" s="6">
+        <v>150</v>
+      </c>
+      <c r="E7" s="8">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45339</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6">
-        <v>150</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
+        <v>150</v>
+      </c>
+      <c r="E8" s="8">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45340</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9">
+      <c r="D9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9">
         <v>1000</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45344</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6">
-        <v>150</v>
-      </c>
-      <c r="D10" s="8">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D10" s="6">
+        <v>150</v>
+      </c>
+      <c r="E10" s="8">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45354</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="6">
+      <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="D11" s="8">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="8">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
         <v>19</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45358</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="6">
         <v>0</v>
       </c>
-      <c r="D12" s="8">
-        <v>30</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="8">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45368</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="6">
-        <v>150</v>
-      </c>
-      <c r="D13" s="8">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D13" s="6">
+        <v>150</v>
+      </c>
+      <c r="E13" s="8">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45371</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="6">
-        <v>150</v>
-      </c>
-      <c r="D14" s="8">
-        <v>30</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="D14" s="6">
+        <v>150</v>
+      </c>
+      <c r="E14" s="8">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
         <v>21</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45383</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2">
+        <v>45383</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="6">
-        <v>150</v>
-      </c>
-      <c r="D15" s="8">
-        <v>30</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" s="6">
+        <v>150</v>
+      </c>
+      <c r="E15" s="8">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
         <v>26</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45386</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D16" s="6">
         <v>0</v>
       </c>
-      <c r="D16" s="8">
-        <v>30</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="8">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45392</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2">
+        <v>45383</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="6">
+      <c r="D17" s="6">
         <v>0</v>
       </c>
-      <c r="D17" s="8">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="8">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
         <v>26</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45400</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="6">
-        <v>150</v>
-      </c>
-      <c r="D18" s="8">
-        <v>30</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D18" s="6">
+        <v>150</v>
+      </c>
+      <c r="E18" s="8">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
         <v>28</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45403</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="6">
-        <v>150</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="D19" s="6">
+        <v>150</v>
+      </c>
+      <c r="E19" s="8">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>29</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45412</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="6">
-        <v>150</v>
-      </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
+        <v>150</v>
+      </c>
+      <c r="E20" s="8">
         <v>50</v>
       </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
       <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>45415</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="6">
+      <c r="D21" s="6">
         <v>100</v>
       </c>
-      <c r="D21" s="8">
-        <v>30</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
+      <c r="E21" s="8">
+        <v>30</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>45418</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="3">
-        <v>150</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="D22" s="6"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="3">
+        <v>150</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45431</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="6">
+      <c r="D23" s="6">
         <v>200</v>
       </c>
-      <c r="D23" s="8">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E23" s="8">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
         <v>33</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45435</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="6">
-        <v>150</v>
-      </c>
-      <c r="D24" s="8">
-        <v>30</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D24" s="6">
+        <v>150</v>
+      </c>
+      <c r="E24" s="8">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
         <v>34</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45438</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="6">
+      <c r="D25" s="6">
         <v>0</v>
       </c>
-      <c r="D25" s="8">
-        <v>30</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25" s="8">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
         <v>32</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45512</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="6">
+      <c r="D26" s="6">
         <v>0</v>
       </c>
-      <c r="D26" s="8">
-        <v>30</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="8">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
         <v>124</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45543</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C27" s="6">
+      <c r="D27" s="6">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>30</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
         <v>162</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45555</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="6">
-        <v>150</v>
-      </c>
-      <c r="D28" s="8">
-        <v>30</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="D28" s="6">
+        <v>150</v>
+      </c>
+      <c r="E28" s="8">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
         <v>126</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45557</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C29" s="6">
-        <v>150</v>
-      </c>
-      <c r="D29" s="8">
-        <v>30</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="D29" s="6">
+        <v>150</v>
+      </c>
+      <c r="E29" s="8">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
         <v>128</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45562</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="6">
+      <c r="D30" s="6">
         <v>80</v>
       </c>
-      <c r="D30" s="8">
+      <c r="E30" s="8">
         <v>40</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>130</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45571</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="6">
-        <v>150</v>
-      </c>
-      <c r="D31" s="8">
-        <v>30</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="D31" s="6">
+        <v>150</v>
+      </c>
+      <c r="E31" s="8">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
         <v>132</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45576</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2">
+        <v>45576</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="6">
-        <v>150</v>
-      </c>
-      <c r="D32" s="8">
+      <c r="D32" s="6">
+        <v>150</v>
+      </c>
+      <c r="E32" s="8">
         <v>50</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>134</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45577</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2">
+        <v>45576</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="6">
-        <v>150</v>
-      </c>
-      <c r="D33" s="8">
+      <c r="D33" s="6">
+        <v>150</v>
+      </c>
+      <c r="E33" s="8">
         <v>50</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>134</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45578</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="6">
-        <v>150</v>
-      </c>
-      <c r="D34" s="8">
+      <c r="D34" s="6">
+        <v>150</v>
+      </c>
+      <c r="E34" s="8">
         <v>50</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>136</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45583</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="6">
-        <v>150</v>
-      </c>
-      <c r="D35" s="8">
-        <v>30</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="D35" s="6">
+        <v>150</v>
+      </c>
+      <c r="E35" s="8">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
         <v>138</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45590</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="6">
+      <c r="D36" s="6">
         <v>200</v>
       </c>
-      <c r="D36" s="8">
-        <v>30</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E36" s="8">
+        <v>30</v>
+      </c>
+      <c r="G36" t="s">
         <v>140</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45599</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="6">
-        <v>150</v>
-      </c>
-      <c r="D37" s="8">
-        <v>30</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="D37" s="6">
+        <v>150</v>
+      </c>
+      <c r="E37" s="8">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
         <v>142</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45604</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C38" s="6">
-        <v>150</v>
-      </c>
-      <c r="D38" s="8">
-        <v>30</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="D38" s="6">
+        <v>150</v>
+      </c>
+      <c r="E38" s="8">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
         <v>144</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45606</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="6">
-        <v>150</v>
-      </c>
-      <c r="D39" s="8">
-        <v>30</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="D39" s="6">
+        <v>150</v>
+      </c>
+      <c r="E39" s="8">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
         <v>146</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45625</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="F40" t="s">
+      <c r="D40" s="6"/>
+      <c r="E40" s="8"/>
+      <c r="G40" t="s">
         <v>148</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45626</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="F41" t="s">
-        <v>150</v>
-      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="8"/>
       <c r="G41" t="s">
+        <v>150</v>
+      </c>
+      <c r="H41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45633</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C42" s="6">
-        <v>150</v>
-      </c>
-      <c r="D42" s="8">
-        <v>30</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="D42" s="6">
+        <v>150</v>
+      </c>
+      <c r="E42" s="8">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
         <v>154</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45634</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="6">
-        <v>150</v>
-      </c>
-      <c r="D43" s="8">
-        <v>30</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="D43" s="6">
+        <v>150</v>
+      </c>
+      <c r="E43" s="8">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
         <v>152</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45641</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="11"/>
-      <c r="F44" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="11"/>
+      <c r="G44" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>45646</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C45" s="6">
-        <v>150</v>
-      </c>
-      <c r="D45" s="8">
-        <v>30</v>
-      </c>
-      <c r="E45" s="10"/>
-      <c r="F45" t="s">
+      <c r="D45" s="6">
+        <v>150</v>
+      </c>
+      <c r="E45" s="8">
+        <v>30</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" t="s">
         <v>157</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2010,7 +2079,7 @@
           <x14:formula1>
             <xm:f>'Kinoförderer gratis'!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G296</xm:sqref>
+          <xm:sqref>G46:G296 H2:H45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2023,19 +2092,19 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2052,7 +2121,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -2069,7 +2138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
@@ -2086,7 +2155,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
@@ -2103,7 +2172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>83</v>
       </c>
@@ -2120,7 +2189,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -2137,7 +2206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
@@ -2154,7 +2223,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
@@ -2171,7 +2240,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -2188,7 +2257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
@@ -2205,7 +2274,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -2222,7 +2291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
@@ -2239,7 +2308,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>48</v>
       </c>
@@ -2256,7 +2325,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -2273,7 +2342,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -2290,7 +2359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -2307,7 +2376,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
@@ -2324,7 +2393,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
@@ -2341,7 +2410,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -2358,7 +2427,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>103</v>
       </c>
@@ -2375,7 +2444,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>119</v>
       </c>
@@ -2392,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>158</v>
       </c>
@@ -2409,7 +2478,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>159</v>
       </c>
@@ -2455,22 +2524,22 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>

</xml_diff>